<commit_message>
docs: update script and lookup table for vehicles
</commit_message>
<xml_diff>
--- a/data-raw/reformatted_Code table_v1.xlsx
+++ b/data-raw/reformatted_Code table_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin Chan\Documents\SourceTree Repos\hkdatasets\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16554D75-31D0-4D4D-B640-F58919473472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F5C5DE-B5E1-4948-99B9-0FEE279F604A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="1395" windowWidth="7020" windowHeight="11910" tabRatio="815" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="10890" tabRatio="815" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Within_70m" sheetId="5" r:id="rId1"/>
@@ -19,27 +19,29 @@
     <sheet name="Road_class_L" sheetId="17" r:id="rId4"/>
     <sheet name="Overtaking" sheetId="8" r:id="rId5"/>
     <sheet name="Main_vehic" sheetId="9" r:id="rId6"/>
-    <sheet name="Vehicle_co" sheetId="10" r:id="rId7"/>
-    <sheet name="First_poin" sheetId="11" r:id="rId8"/>
-    <sheet name="Ped_Location" sheetId="12" r:id="rId9"/>
-    <sheet name="Ped_Special" sheetId="13" r:id="rId10"/>
-    <sheet name="Ped_Action" sheetId="18" r:id="rId11"/>
-    <sheet name="A1_street_name" sheetId="4" r:id="rId12"/>
-    <sheet name="Ped_Cycle" sheetId="14" r:id="rId13"/>
-    <sheet name="Collision_Type" sheetId="15" r:id="rId14"/>
-    <sheet name="Struc_Type" sheetId="16" r:id="rId15"/>
+    <sheet name="Vehicle_Class" sheetId="19" r:id="rId7"/>
+    <sheet name="Vehicle_co" sheetId="10" r:id="rId8"/>
+    <sheet name="First_poin" sheetId="11" r:id="rId9"/>
+    <sheet name="Ped_Location" sheetId="12" r:id="rId10"/>
+    <sheet name="Ped_Special" sheetId="13" r:id="rId11"/>
+    <sheet name="Ped_Action" sheetId="18" r:id="rId12"/>
+    <sheet name="Sev_of" sheetId="20" r:id="rId13"/>
+    <sheet name="A1_street_name" sheetId="4" r:id="rId14"/>
+    <sheet name="Ped_Cycle" sheetId="14" r:id="rId15"/>
+    <sheet name="Collision_Type" sheetId="15" r:id="rId16"/>
+    <sheet name="Struc_Type" sheetId="16" r:id="rId17"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId16" roundtripDataSignature="AMtx7mifERmNh4aE2Y1wURIPXNkdZj8iJw=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId18" roundtripDataSignature="AMtx7mifERmNh4aE2Y1wURIPXNkdZj8iJw=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4867" uniqueCount="4748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4887" uniqueCount="4764">
   <si>
     <t>Code</t>
   </si>
@@ -14283,6 +14285,66 @@
   </si>
   <si>
     <t>Not known</t>
+  </si>
+  <si>
+    <t>Motorcycle</t>
+  </si>
+  <si>
+    <t>Private car</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Public light bus</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Light goods vehicle</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Medium goods vehicle</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heavy goods vehicle</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Public franchised bus</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Public non-franchised bus</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taxi</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bicycle</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tram</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Light rail vehicle</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Others (incl. unknown)</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fatal</t>
+  </si>
+  <si>
+    <t>Serious</t>
+  </si>
+  <si>
+    <t>Slight</t>
   </si>
 </sst>
 </file>
@@ -14582,6 +14644,93 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C99ED95-B70D-46E4-8942-443CF74C5091}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V24" sqref="V24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4712</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F32E334-A2C9-4EF5-B13B-EB3ADBE9DC13}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -14668,12 +14817,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33CEBD57-7D7A-435C-854D-A0DF5C621E03}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14788,7 +14937,54 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0331BA88-A9C9-49D4-94B0-D4B4069BCB96}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4712</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4761</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4762</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4763</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B4723"/>
   <sheetViews>
@@ -52593,7 +52789,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB665CB8-71FF-E940-90AD-89581B11B154}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -52640,7 +52836,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3E75C0E-BB4D-7C4A-95C9-C696687FB968}">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -52735,7 +52931,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E76B1F9-618B-404B-9245-2AC93B9C2359}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -53063,7 +53259,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B21"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -53242,11 +53438,141 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF8616A-58F7-4361-8209-017220062387}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4712</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4748</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4749</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4750</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4751</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4752</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4753</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4754</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4755</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4756</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4757</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4758</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4759</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4760</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42E64ACC-F596-4CB7-9809-F7546110AF6B}">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+      <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -53432,7 +53758,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C79AEB-CD41-4832-9E5A-9C3B0EC67E86}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -53501,91 +53827,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C99ED95-B70D-46E4-8942-443CF74C5091}">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V24" sqref="V24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4712</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>